<commit_message>
Presented best_topic and matching_overarching column, also new worksheet. Switched to openpyxl
</commit_message>
<xml_diff>
--- a/Column_Setup.xlsx
+++ b/Column_Setup.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gandr\Desktop\College Classes\Spring 2019 Classes\AI\LDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\gandr\Documents\GitHub\LDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EA6283-AD46-48E0-A739-19690C999073}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBF05A6-4ABB-4B56-BEF6-5B689E322EDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0C0C7323-D074-4B97-995B-BB4B0EE5946B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>Tom sailed the high seas looking for new lands to conquer. Is that land off in the distance?</t>
+  </si>
+  <si>
+    <t>Best_Topic</t>
+  </si>
+  <si>
+    <t>Matching_Overarching</t>
   </si>
 </sst>
 </file>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAEB9F9-12D9-46D3-A301-15C404858E8C}">
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AJ1" sqref="AJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,9 +574,10 @@
     <col min="5" max="21" width="21.5546875" customWidth="1"/>
     <col min="22" max="27" width="21.6640625" customWidth="1"/>
     <col min="28" max="35" width="22.109375" customWidth="1"/>
+    <col min="36" max="36" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -673,8 +680,14 @@
       <c r="AH1" t="s">
         <v>33</v>
       </c>
+      <c r="AI1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -688,7 +701,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -702,7 +715,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -716,7 +729,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -730,7 +743,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -744,7 +757,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -758,7 +771,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -772,7 +785,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>

</xml_diff>